<commit_message>
Text now added to .xlsx when /bug
</commit_message>
<xml_diff>
--- a/tracking/vCGP Tracking Document.xlsx
+++ b/tracking/vCGP Tracking Document.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B925384-97C9-417D-90FC-43E43C71E493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{7B925384-97C9-417D-90FC-43E43C71E493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{756A2337-0C96-4BD8-A9CD-43FE477EBDC1}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Features</t>
   </si>
@@ -54,17 +57,74 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Statused</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Release Version</t>
+  </si>
+  <si>
+    <t>Attachments</t>
+  </si>
+  <si>
     <t>Resolved</t>
   </si>
   <si>
-    <t>Attachments</t>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Make DCB transparent</t>
+  </si>
+  <si>
+    <t>I think the DCB should be transparent so you can still see targetes under it</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>v1.2.3</t>
+  </si>
+  <si>
+    <t>DCB not showing</t>
+  </si>
+  <si>
+    <t>The DCB doesn't appear    test test test test test when I start the app</t>
+  </si>
+  <si>
+    <t>cdn.discord.com/12345678</t>
+  </si>
+  <si>
+    <t>Declined</t>
+  </si>
+  <si>
+    <t>v3.20.1</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>9/172023</t>
+  </si>
+  <si>
+    <t>v1.2.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +132,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +187,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -174,55 +281,150 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,154 +744,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:W3"/>
+  <dimension ref="B1:Z6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.140625" style="11"/>
-    <col min="3" max="3" width="18.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="11" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="9.140625" style="11"/>
-    <col min="10" max="10" width="18.7109375" style="11" customWidth="1"/>
-    <col min="11" max="12" width="23.140625" style="11" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" style="11" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="11"/>
-    <col min="18" max="18" width="18.7109375" style="11" customWidth="1"/>
-    <col min="19" max="20" width="23.140625" style="11" customWidth="1"/>
-    <col min="21" max="22" width="12.7109375" style="11" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="33"/>
+    <col min="12" max="12" width="18.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="12.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="33"/>
+    <col min="21" max="21" width="18.7109375" style="2" customWidth="1"/>
+    <col min="22" max="23" width="23.140625" style="2" customWidth="1"/>
+    <col min="24" max="25" width="12.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23">
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+    <row r="1" spans="2:26">
+      <c r="B1" s="30"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="14"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="2:23">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:26">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="I2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
-      <c r="Q2" s="8" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="T2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="10"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="13"/>
     </row>
-    <row r="3" spans="2:23">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:26">
+      <c r="B3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" s="28" customFormat="1" ht="14.25" customHeight="1">
+      <c r="B4" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="20">
+        <v>47371</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="20">
+        <v>45179</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="25">
+        <v>45179</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>45179</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="35"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+    </row>
+    <row r="5" spans="2:26" ht="15.75" customHeight="1">
+      <c r="B5" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="25">
+        <v>47371</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="25">
+        <v>45182</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="15" customHeight="1">
+      <c r="B6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="41">
+        <v>47371</v>
+      </c>
+      <c r="F6" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>8</v>
+      <c r="G6" s="41">
+        <v>45183</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="T2:Z2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{C6EE4EE6-05BB-41CD-A067-D3BCD459A1D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>